<commit_message>
some pattern checker and some kbts on this branch
</commit_message>
<xml_diff>
--- a/charts_xlsx/cschart.xlsx
+++ b/charts_xlsx/cschart.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="327">
   <si>
     <t>Sign Degree: [Planet]</t>
   </si>
@@ -208,6 +208,9 @@
     <t xml:space="preserve">0: [JUPITER] </t>
   </si>
   <si>
+    <t xml:space="preserve">PEREGRINE: [0] </t>
+  </si>
+  <si>
     <t xml:space="preserve">0: [-2 SEPARATING SEMISEXTILE to SATURN; 2 APPLYING SEXTILE to NEPTUNE] </t>
   </si>
   <si>
@@ -253,6 +256,9 @@
     <t xml:space="preserve">28: [SATURN] </t>
   </si>
   <si>
+    <t xml:space="preserve">FALL: [3] </t>
+  </si>
+  <si>
     <t xml:space="preserve">28: [-2 APPLYING SEXTILE to SUN; 1 APPLYING SEMISQUARE to ASC; 9 SEPARATING OPPOSITION to MARS; -2 SEPARATING SEMISEXTILE to JUPITER; 4 APPLYING SQUARE to NEPTUNE] </t>
   </si>
   <si>
@@ -352,11 +358,9 @@
     <t xml:space="preserve">74: [6 SEPARATING TRINE to MOON; 8 SEPARATING SQUARE to VENUS; -1 APPLYING BIQUINTILE to MARS; 1 APPLYING SEMISQUARE to SATURN; -1 APPLYING TRINE to URANUS; -4 APPLYING OPPOSITION to PLUTO] </t>
   </si>
   <si>
-    <t>74: [STITCH DETERMINER FOR: SEPARATING TRINE (ASC, MOON) [Score:Intensity: TRINE:8 - Exactness:6, Calc Score:2] 
-Diamonds, Triangles, or Leaves 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Planet Scores: 0, 11 
- Orb Width: 8]</t>
+    <t>74: [[&lt;PatternStitchBase.PURL: 0&gt;, &lt;PatternStitchBase.PURL: 0&gt;] in Ptbl 
+  for 4 stitches on the WS over 8 stitches 
+  Aspecting Planet Dignity Scores: 0, 10]</t>
   </si>
   <si>
     <t>75</t>
@@ -650,6 +654,9 @@
     <t xml:space="preserve">217: [MARS] </t>
   </si>
   <si>
+    <t xml:space="preserve">RULERSHIP: [8] </t>
+  </si>
+  <si>
     <t xml:space="preserve">217: [-1 APPLYING BIQUINTILE to ASC; -2 APPLYING TRINE to MERCURY; 9 SEPARATING OPPOSITION to SATURN; 6 APPLYING SQUARE to URANUS; -5 SEPARATING SQUARE to NEPTUNE] </t>
   </si>
   <si>
@@ -830,6 +837,9 @@
     <t xml:space="preserve">302: [NEPTUNE] </t>
   </si>
   <si>
+    <t xml:space="preserve">PEREGRINE: [1] </t>
+  </si>
+  <si>
     <t xml:space="preserve">302: [-5 SEPARATING SQUARE to MARS; 2 APPLYING SEXTILE to JUPITER; 4 APPLYING SQUARE to SATURN] </t>
   </si>
   <si>
@@ -878,21 +888,14 @@
     <t xml:space="preserve">320: [MOON] </t>
   </si>
   <si>
-    <t xml:space="preserve">PEREGRINE: [1] </t>
-  </si>
-  <si>
     <t xml:space="preserve">320: [6 APPLYING CONJ to SUN; 6 SEPARATING TRINE to ASC; 2 APPLYING SEMISEXTILE to VENUS; 7 SEPARATING CONJ to URANUS] </t>
   </si>
   <si>
-    <t>320: [STITCH DETERMINER FOR: APPLYING CONJ (MOON, SUN) [Score:Intensity: CONJ:10 - Exactness:6, Calc Score:4] 
-Lines, circles, or Chains 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Planet Scores: 11, 11 
- Orb Width: 10; STITCH DETERMINER FOR: SEPARATING TRINE (MOON, ASC) [Score:Intensity: TRINE:8 - Exactness:6, Calc Score:2] 
-Diamonds, Triangles, or Leaves 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Planet Scores: 11, 0 
- Orb Width: 8]</t>
+    <t>320: [[&lt;PatternStitchBase.PURL: 0&gt;, &lt;PatternStitchBase.PURL: 0&gt;] in YO, M1L, M1R 
+  for 4 stitches on the RS over 10 stitches 
+  Aspecting Planet Dignity Scores: 10, 11; [&lt;PatternStitchBase.PURL: 0&gt;, &lt;PatternStitchBase.PURL: 0&gt;] in Ptbl 
+  for 4 stitches on the WS over 8 stitches 
+  Aspecting Planet Dignity Scores: 10, 0]</t>
   </si>
   <si>
     <t>321</t>
@@ -916,11 +919,9 @@
     <t xml:space="preserve">326: [6 APPLYING CONJ to MOON; 9 SEPARATING CONJ to MERCURY; -2 APPLYING SEXTILE to SATURN] </t>
   </si>
   <si>
-    <t>326: [STITCH DETERMINER FOR: APPLYING CONJ (SUN, MOON) [Score:Intensity: CONJ:10 - Exactness:6, Calc Score:4] 
-Lines, circles, or Chains 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Planet Scores: 11, 11 
- Orb Width: 10]</t>
+    <t>326: [[&lt;PatternStitchBase.PURL: 0&gt;, &lt;PatternStitchBase.PURL: 0&gt;] in YO, M1L, M1R 
+  for 4 stitches on the RS over 10 stitches 
+  Aspecting Planet Dignity Scores: 11, 10]</t>
   </si>
   <si>
     <t>327</t>
@@ -984,6 +985,9 @@
   </si>
   <si>
     <t xml:space="preserve">352: [VENUS] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXHAULTATION: [5] </t>
   </si>
   <si>
     <t xml:space="preserve">352: [2 APPLYING SEMISEXTILE to MOON; 8 SEPARATING SQUARE to ASC] </t>
@@ -1468,8 +1472,11 @@
       <c r="B2" t="s">
         <v>63</v>
       </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>62</v>
@@ -1487,7 +1494,7 @@
     </row>
     <row r="3" spans="2:34">
       <c r="E3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -1508,7 +1515,7 @@
     </row>
     <row r="4" spans="2:34">
       <c r="E4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -1535,7 +1542,7 @@
     </row>
     <row r="5" spans="2:34">
       <c r="E5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
@@ -1562,7 +1569,7 @@
     </row>
     <row r="6" spans="2:34">
       <c r="E6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
@@ -1595,7 +1602,7 @@
     </row>
     <row r="7" spans="2:34">
       <c r="E7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
         <v>29</v>
@@ -1622,10 +1629,10 @@
     </row>
     <row r="8" spans="2:34">
       <c r="E8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" t="s">
         <v>71</v>
-      </c>
-      <c r="F8" t="s">
-        <v>70</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>33</v>
@@ -1655,10 +1662,10 @@
     </row>
     <row r="9" spans="2:34">
       <c r="E9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
         <v>73</v>
-      </c>
-      <c r="F9" t="s">
-        <v>72</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>33</v>
@@ -1682,10 +1689,10 @@
     </row>
     <row r="10" spans="2:34">
       <c r="E10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" t="s">
         <v>75</v>
-      </c>
-      <c r="F10" t="s">
-        <v>74</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>33</v>
@@ -1709,16 +1716,19 @@
     </row>
     <row r="11" spans="2:34">
       <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" t="s">
         <v>78</v>
       </c>
-      <c r="D11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>77</v>
-      </c>
-      <c r="F11" t="s">
-        <v>76</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>33</v>
@@ -1736,10 +1746,10 @@
     </row>
     <row r="12" spans="2:34">
       <c r="E12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>33</v>
@@ -1763,10 +1773,10 @@
     </row>
     <row r="13" spans="2:34">
       <c r="E13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M13">
         <f>SUM(J12:L12)</f>
@@ -1778,10 +1788,10 @@
     </row>
     <row r="14" spans="2:34">
       <c r="E14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>35</v>
@@ -1799,10 +1809,10 @@
     </row>
     <row r="15" spans="2:34">
       <c r="E15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="M15">
         <f>SUM(J14:L14)</f>
@@ -1814,10 +1824,10 @@
     </row>
     <row r="16" spans="2:34">
       <c r="E16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>46</v>
@@ -1841,10 +1851,10 @@
     </row>
     <row r="17" spans="2:17">
       <c r="E17" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>46</v>
@@ -1868,10 +1878,10 @@
     </row>
     <row r="18" spans="2:17">
       <c r="E18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>36</v>
@@ -1895,10 +1905,10 @@
     </row>
     <row r="19" spans="2:17">
       <c r="E19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>36</v>
@@ -1922,10 +1932,10 @@
     </row>
     <row r="20" spans="2:17">
       <c r="E20" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F20" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>36</v>
@@ -1949,10 +1959,10 @@
     </row>
     <row r="21" spans="2:17">
       <c r="E21" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F21" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>36</v>
@@ -1976,10 +1986,10 @@
     </row>
     <row r="22" spans="2:17">
       <c r="E22" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F22" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>36</v>
@@ -1997,10 +2007,10 @@
     </row>
     <row r="23" spans="2:17">
       <c r="E23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>36</v>
@@ -2024,10 +2034,10 @@
     </row>
     <row r="24" spans="2:17">
       <c r="E24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>51</v>
@@ -2045,10 +2055,10 @@
     </row>
     <row r="25" spans="2:17">
       <c r="E25" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F25" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>51</v>
@@ -2066,16 +2076,16 @@
     </row>
     <row r="26" spans="2:17">
       <c r="B26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" t="s">
         <v>110</v>
-      </c>
-      <c r="D26" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" t="s">
-        <v>108</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>47</v>
@@ -2094,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="Q26">
         <v>25</v>
@@ -2102,10 +2112,10 @@
     </row>
     <row r="27" spans="2:17">
       <c r="E27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F27" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>47</v>
@@ -2129,10 +2139,10 @@
     </row>
     <row r="28" spans="2:17">
       <c r="E28" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F28" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>37</v>
@@ -2162,10 +2172,10 @@
     </row>
     <row r="29" spans="2:17">
       <c r="E29" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F29" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>37</v>
@@ -2195,10 +2205,10 @@
     </row>
     <row r="30" spans="2:17">
       <c r="E30" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F30" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>37</v>
@@ -2222,10 +2232,10 @@
     </row>
     <row r="31" spans="2:17">
       <c r="E31" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F31" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>37</v>
@@ -2249,10 +2259,10 @@
     </row>
     <row r="32" spans="2:17">
       <c r="E32" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F32" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>37</v>
@@ -2270,10 +2280,10 @@
     </row>
     <row r="33" spans="5:17">
       <c r="E33" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F33" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>37</v>
@@ -2291,10 +2301,10 @@
     </row>
     <row r="34" spans="5:17">
       <c r="E34" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="M34">
         <f>SUM(J33:L33)</f>
@@ -2306,10 +2316,10 @@
     </row>
     <row r="35" spans="5:17">
       <c r="E35" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F35" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="M35">
         <f>SUM(J34:L34)</f>
@@ -2321,10 +2331,10 @@
     </row>
     <row r="36" spans="5:17">
       <c r="E36" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F36" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>48</v>
@@ -2348,10 +2358,10 @@
     </row>
     <row r="37" spans="5:17">
       <c r="E37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F37" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>52</v>
@@ -2369,10 +2379,10 @@
     </row>
     <row r="38" spans="5:17">
       <c r="E38" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F38" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>38</v>
@@ -2396,10 +2406,10 @@
     </row>
     <row r="39" spans="5:17">
       <c r="E39" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F39" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>49</v>
@@ -2417,10 +2427,10 @@
     </row>
     <row r="40" spans="5:17">
       <c r="E40" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F40" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>39</v>
@@ -2438,10 +2448,10 @@
     </row>
     <row r="41" spans="5:17">
       <c r="E41" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F41" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>39</v>
@@ -2465,10 +2475,10 @@
     </row>
     <row r="42" spans="5:17">
       <c r="E42" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F42" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>54</v>
@@ -2486,10 +2496,10 @@
     </row>
     <row r="43" spans="5:17">
       <c r="E43" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F43" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="M43">
         <f>SUM(J42:L42)</f>
@@ -2501,10 +2511,10 @@
     </row>
     <row r="44" spans="5:17">
       <c r="E44" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F44" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>53</v>
@@ -2522,10 +2532,10 @@
     </row>
     <row r="45" spans="5:17">
       <c r="E45" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F45" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>50</v>
@@ -2549,10 +2559,10 @@
     </row>
     <row r="46" spans="5:17">
       <c r="E46" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F46" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>50</v>
@@ -2576,10 +2586,10 @@
     </row>
     <row r="47" spans="5:17">
       <c r="E47" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F47" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>40</v>
@@ -2609,10 +2619,10 @@
     </row>
     <row r="48" spans="5:17">
       <c r="E48" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F48" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>40</v>
@@ -2642,10 +2652,10 @@
     </row>
     <row r="49" spans="5:17">
       <c r="E49" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F49" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>40</v>
@@ -2669,10 +2679,10 @@
     </row>
     <row r="50" spans="5:17">
       <c r="E50" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F50" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>40</v>
@@ -2702,10 +2712,10 @@
     </row>
     <row r="51" spans="5:17">
       <c r="E51" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F51" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>40</v>
@@ -2729,10 +2739,10 @@
     </row>
     <row r="52" spans="5:17">
       <c r="E52" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F52" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>40</v>
@@ -2750,10 +2760,10 @@
     </row>
     <row r="53" spans="5:17">
       <c r="E53" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F53" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>40</v>
@@ -2771,10 +2781,10 @@
     </row>
     <row r="54" spans="5:17">
       <c r="E54" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F54" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>56</v>
@@ -2792,10 +2802,10 @@
     </row>
     <row r="55" spans="5:17">
       <c r="E55" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F55" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="I55" s="3" t="s">
         <v>56</v>
@@ -2813,10 +2823,10 @@
     </row>
     <row r="56" spans="5:17">
       <c r="E56" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F56" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>56</v>
@@ -2834,10 +2844,10 @@
     </row>
     <row r="57" spans="5:17">
       <c r="E57" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F57" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>56</v>
@@ -2855,10 +2865,10 @@
     </row>
     <row r="58" spans="5:17">
       <c r="E58" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F58" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>49</v>
@@ -2882,10 +2892,10 @@
     </row>
     <row r="59" spans="5:17">
       <c r="E59" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F59" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>49</v>
@@ -2909,10 +2919,10 @@
     </row>
     <row r="60" spans="5:17">
       <c r="E60" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F60" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>39</v>
@@ -2930,10 +2940,10 @@
     </row>
     <row r="61" spans="5:17">
       <c r="E61" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F61" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>39</v>
@@ -2951,10 +2961,10 @@
     </row>
     <row r="62" spans="5:17">
       <c r="E62" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F62" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="M62">
         <f>SUM(J61:L61)</f>
@@ -2966,10 +2976,10 @@
     </row>
     <row r="63" spans="5:17">
       <c r="E63" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F63" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="M63">
         <f>SUM(J62:L62)</f>
@@ -2981,10 +2991,10 @@
     </row>
     <row r="64" spans="5:17">
       <c r="E64" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="F64" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I64" s="3" t="s">
         <v>57</v>
@@ -3002,10 +3012,10 @@
     </row>
     <row r="65" spans="2:17">
       <c r="E65" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F65" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I65" s="3" t="s">
         <v>57</v>
@@ -3023,10 +3033,10 @@
     </row>
     <row r="66" spans="2:17">
       <c r="E66" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F66" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>47</v>
@@ -3050,10 +3060,10 @@
     </row>
     <row r="67" spans="2:17">
       <c r="E67" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F67" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>47</v>
@@ -3077,10 +3087,10 @@
     </row>
     <row r="68" spans="2:17">
       <c r="E68" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F68" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>37</v>
@@ -3110,10 +3120,10 @@
     </row>
     <row r="69" spans="2:17">
       <c r="E69" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F69" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>37</v>
@@ -3143,10 +3153,10 @@
     </row>
     <row r="70" spans="2:17">
       <c r="E70" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F70" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>37</v>
@@ -3170,10 +3180,10 @@
     </row>
     <row r="71" spans="2:17">
       <c r="E71" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F71" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>37</v>
@@ -3197,10 +3207,10 @@
     </row>
     <row r="72" spans="2:17">
       <c r="E72" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F72" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>37</v>
@@ -3218,10 +3228,10 @@
     </row>
     <row r="73" spans="2:17">
       <c r="E73" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F73" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>37</v>
@@ -3239,16 +3249,19 @@
     </row>
     <row r="74" spans="2:17">
       <c r="B74" t="s">
+        <v>211</v>
+      </c>
+      <c r="C74" t="s">
+        <v>212</v>
+      </c>
+      <c r="D74" t="s">
+        <v>213</v>
+      </c>
+      <c r="E74" t="s">
+        <v>210</v>
+      </c>
+      <c r="F74" t="s">
         <v>209</v>
-      </c>
-      <c r="D74" t="s">
-        <v>210</v>
-      </c>
-      <c r="E74" t="s">
-        <v>208</v>
-      </c>
-      <c r="F74" t="s">
-        <v>207</v>
       </c>
       <c r="I74" s="3" t="s">
         <v>58</v>
@@ -3266,10 +3279,10 @@
     </row>
     <row r="75" spans="2:17">
       <c r="E75" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F75" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="M75">
         <f>SUM(J74:L74)</f>
@@ -3281,10 +3294,10 @@
     </row>
     <row r="76" spans="2:17">
       <c r="E76" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F76" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>46</v>
@@ -3308,10 +3321,10 @@
     </row>
     <row r="77" spans="2:17">
       <c r="E77" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="F77" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>46</v>
@@ -3335,10 +3348,10 @@
     </row>
     <row r="78" spans="2:17">
       <c r="E78" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F78" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>36</v>
@@ -3362,10 +3375,10 @@
     </row>
     <row r="79" spans="2:17">
       <c r="E79" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F79" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>36</v>
@@ -3389,10 +3402,10 @@
     </row>
     <row r="80" spans="2:17">
       <c r="E80" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F80" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>36</v>
@@ -3416,10 +3429,10 @@
     </row>
     <row r="81" spans="2:17">
       <c r="E81" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F81" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>36</v>
@@ -3443,10 +3456,10 @@
     </row>
     <row r="82" spans="2:17">
       <c r="E82" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="F82" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>36</v>
@@ -3464,10 +3477,10 @@
     </row>
     <row r="83" spans="2:17">
       <c r="E83" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F83" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>36</v>
@@ -3491,10 +3504,10 @@
     </row>
     <row r="84" spans="2:17">
       <c r="E84" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F84" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="I84" s="3" t="s">
         <v>60</v>
@@ -3512,16 +3525,19 @@
     </row>
     <row r="85" spans="2:17">
       <c r="B85" t="s">
-        <v>233</v>
+        <v>236</v>
+      </c>
+      <c r="C85" t="s">
+        <v>64</v>
       </c>
       <c r="D85" t="s">
+        <v>237</v>
+      </c>
+      <c r="E85" t="s">
+        <v>235</v>
+      </c>
+      <c r="F85" t="s">
         <v>234</v>
-      </c>
-      <c r="E85" t="s">
-        <v>232</v>
-      </c>
-      <c r="F85" t="s">
-        <v>231</v>
       </c>
       <c r="I85" s="3" t="s">
         <v>60</v>
@@ -3539,10 +3555,10 @@
     </row>
     <row r="86" spans="2:17">
       <c r="E86" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F86" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>43</v>
@@ -3566,10 +3582,10 @@
     </row>
     <row r="87" spans="2:17">
       <c r="E87" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F87" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>43</v>
@@ -3593,10 +3609,10 @@
     </row>
     <row r="88" spans="2:17">
       <c r="E88" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F88" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>33</v>
@@ -3626,10 +3642,10 @@
     </row>
     <row r="89" spans="2:17">
       <c r="E89" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F89" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>33</v>
@@ -3659,10 +3675,10 @@
     </row>
     <row r="90" spans="2:17">
       <c r="E90" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F90" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>33</v>
@@ -3686,10 +3702,10 @@
     </row>
     <row r="91" spans="2:17">
       <c r="E91" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F91" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>33</v>
@@ -3707,10 +3723,10 @@
     </row>
     <row r="92" spans="2:17">
       <c r="E92" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F92" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="G92" s="4" t="s">
         <v>33</v>
@@ -3728,10 +3744,10 @@
     </row>
     <row r="93" spans="2:17">
       <c r="E93" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F93" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="M93">
         <f>SUM(J92:L92)</f>
@@ -3743,10 +3759,10 @@
     </row>
     <row r="94" spans="2:17">
       <c r="E94" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="F94" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="M94">
         <f>SUM(J93:L93)</f>
@@ -3758,10 +3774,10 @@
     </row>
     <row r="95" spans="2:17">
       <c r="E95" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="F95" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="M95">
         <f>SUM(J94:L94)</f>
@@ -3773,10 +3789,10 @@
     </row>
     <row r="96" spans="2:17">
       <c r="E96" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="F96" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="I96" s="3" t="s">
         <v>59</v>
@@ -3794,10 +3810,10 @@
     </row>
     <row r="97" spans="2:17">
       <c r="E97" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="F97" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="I97" s="3" t="s">
         <v>59</v>
@@ -3815,10 +3831,10 @@
     </row>
     <row r="98" spans="2:17">
       <c r="E98" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F98" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>42</v>
@@ -3836,10 +3852,10 @@
     </row>
     <row r="99" spans="2:17">
       <c r="E99" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="F99" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="H99" s="2" t="s">
         <v>42</v>
@@ -3857,10 +3873,10 @@
     </row>
     <row r="100" spans="2:17">
       <c r="E100" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="F100" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="G100" s="4" t="s">
         <v>32</v>
@@ -3878,10 +3894,10 @@
     </row>
     <row r="101" spans="2:17">
       <c r="E101" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F101" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G101" s="4" t="s">
         <v>32</v>
@@ -3899,16 +3915,19 @@
     </row>
     <row r="102" spans="2:17">
       <c r="B102" t="s">
-        <v>269</v>
+        <v>272</v>
+      </c>
+      <c r="C102" t="s">
+        <v>273</v>
       </c>
       <c r="D102" t="s">
+        <v>274</v>
+      </c>
+      <c r="E102" t="s">
+        <v>271</v>
+      </c>
+      <c r="F102" t="s">
         <v>270</v>
-      </c>
-      <c r="E102" t="s">
-        <v>268</v>
-      </c>
-      <c r="F102" t="s">
-        <v>267</v>
       </c>
       <c r="M102">
         <f>SUM(J101:L101)</f>
@@ -3920,10 +3939,10 @@
     </row>
     <row r="103" spans="2:17">
       <c r="E103" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="F103" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="M103">
         <f>SUM(J102:L102)</f>
@@ -3935,10 +3954,10 @@
     </row>
     <row r="104" spans="2:17">
       <c r="E104" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="F104" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="I104" s="3" t="s">
         <v>57</v>
@@ -3956,10 +3975,10 @@
     </row>
     <row r="105" spans="2:17">
       <c r="E105" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="F105" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="H105" s="2" t="s">
         <v>41</v>
@@ -3983,16 +4002,19 @@
     </row>
     <row r="106" spans="2:17">
       <c r="B106" t="s">
-        <v>279</v>
+        <v>283</v>
+      </c>
+      <c r="C106" t="s">
+        <v>212</v>
       </c>
       <c r="D106" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E106" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="F106" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H106" s="2" t="s">
         <v>41</v>
@@ -4016,10 +4038,10 @@
     </row>
     <row r="107" spans="2:17">
       <c r="E107" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="F107" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="G107" s="4" t="s">
         <v>31</v>
@@ -4049,19 +4071,19 @@
     </row>
     <row r="108" spans="2:17">
       <c r="B108" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C108" t="s">
-        <v>286</v>
+        <v>64</v>
       </c>
       <c r="D108" t="s">
+        <v>290</v>
+      </c>
+      <c r="E108" t="s">
+        <v>288</v>
+      </c>
+      <c r="F108" t="s">
         <v>287</v>
-      </c>
-      <c r="E108" t="s">
-        <v>284</v>
-      </c>
-      <c r="F108" t="s">
-        <v>283</v>
       </c>
       <c r="G108" s="4" t="s">
         <v>31</v>
@@ -4086,7 +4108,7 @@
         <v>0</v>
       </c>
       <c r="P108" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="Q108">
         <v>107</v>
@@ -4094,10 +4116,10 @@
     </row>
     <row r="109" spans="2:17">
       <c r="E109" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="F109" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="G109" s="4" t="s">
         <v>31</v>
@@ -4127,19 +4149,19 @@
     </row>
     <row r="110" spans="2:17">
       <c r="B110" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C110" t="s">
+        <v>297</v>
+      </c>
+      <c r="D110" t="s">
+        <v>298</v>
+      </c>
+      <c r="E110" t="s">
+        <v>295</v>
+      </c>
+      <c r="F110" t="s">
         <v>294</v>
-      </c>
-      <c r="D110" t="s">
-        <v>295</v>
-      </c>
-      <c r="E110" t="s">
-        <v>292</v>
-      </c>
-      <c r="F110" t="s">
-        <v>291</v>
       </c>
       <c r="G110" s="4" t="s">
         <v>31</v>
@@ -4158,7 +4180,7 @@
         <v>0</v>
       </c>
       <c r="P110" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="Q110">
         <v>109</v>
@@ -4166,10 +4188,10 @@
     </row>
     <row r="111" spans="2:17">
       <c r="E111" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="F111" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="G111" s="4" t="s">
         <v>31</v>
@@ -4193,10 +4215,10 @@
     </row>
     <row r="112" spans="2:17">
       <c r="E112" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="F112" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="G112" s="4" t="s">
         <v>31</v>
@@ -4214,16 +4236,19 @@
     </row>
     <row r="113" spans="2:17">
       <c r="B113" t="s">
-        <v>303</v>
+        <v>306</v>
+      </c>
+      <c r="C113" t="s">
+        <v>80</v>
       </c>
       <c r="D113" t="s">
+        <v>307</v>
+      </c>
+      <c r="E113" t="s">
+        <v>305</v>
+      </c>
+      <c r="F113" t="s">
         <v>304</v>
-      </c>
-      <c r="E113" t="s">
-        <v>302</v>
-      </c>
-      <c r="F113" t="s">
-        <v>301</v>
       </c>
       <c r="G113" s="4" t="s">
         <v>31</v>
@@ -4241,10 +4266,10 @@
     </row>
     <row r="114" spans="2:17">
       <c r="E114" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F114" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="I114" s="3" t="s">
         <v>56</v>
@@ -4262,10 +4287,10 @@
     </row>
     <row r="115" spans="2:17">
       <c r="E115" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F115" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I115" s="3" t="s">
         <v>56</v>
@@ -4283,10 +4308,10 @@
     </row>
     <row r="116" spans="2:17">
       <c r="E116" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F116" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I116" s="3" t="s">
         <v>56</v>
@@ -4304,10 +4329,10 @@
     </row>
     <row r="117" spans="2:17">
       <c r="E117" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F117" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="I117" s="3" t="s">
         <v>56</v>
@@ -4325,10 +4350,10 @@
     </row>
     <row r="118" spans="2:17">
       <c r="E118" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F118" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H118" s="2" t="s">
         <v>42</v>
@@ -4352,16 +4377,19 @@
     </row>
     <row r="119" spans="2:17">
       <c r="B119" t="s">
-        <v>317</v>
+        <v>320</v>
+      </c>
+      <c r="C119" t="s">
+        <v>321</v>
       </c>
       <c r="D119" t="s">
+        <v>322</v>
+      </c>
+      <c r="E119" t="s">
+        <v>319</v>
+      </c>
+      <c r="F119" t="s">
         <v>318</v>
-      </c>
-      <c r="E119" t="s">
-        <v>316</v>
-      </c>
-      <c r="F119" t="s">
-        <v>315</v>
       </c>
       <c r="H119" s="2" t="s">
         <v>42</v>
@@ -4385,10 +4413,10 @@
     </row>
     <row r="120" spans="2:17">
       <c r="E120" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="F120" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="G120" s="4" t="s">
         <v>32</v>
@@ -4406,10 +4434,10 @@
     </row>
     <row r="121" spans="2:17">
       <c r="E121" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="F121" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>32</v>

</xml_diff>